<commit_message>
added rpi shield project
</commit_message>
<xml_diff>
--- a/Hardware/ciam/impeller/impeller/BOM_другое.xlsx
+++ b/Hardware/ciam/impeller/impeller/BOM_другое.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yura\Documents\GitHub\Kitties-Hardware\Hardware\ciam\impeller\impeller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A53239-0EF9-42F5-8408-714ACEFB493B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CB972E-D2AD-43D3-86A7-DEA9B11C8998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="13668" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="13620" yWindow="4152" windowWidth="13668" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>